<commit_message>
Changed x value to NA
</commit_message>
<xml_diff>
--- a/inst/extdata/DataExample.xlsx
+++ b/inst/extdata/DataExample.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="20">
   <si>
     <t>meters</t>
   </si>
@@ -154,7 +154,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -184,6 +184,9 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="19" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -495,7 +498,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:O58"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -786,8 +791,8 @@
       <c r="B9" s="4">
         <v>39927.577033310183</v>
       </c>
-      <c r="C9" s="5">
-        <v>-1.4</v>
+      <c r="C9" s="17" t="s">
+        <v>6</v>
       </c>
       <c r="D9" s="5">
         <v>-3.4</v>

</xml_diff>

<commit_message>
Digits replaced with format, still need to deal with export function
</commit_message>
<xml_diff>
--- a/inst/extdata/DataExample.xlsx
+++ b/inst/extdata/DataExample.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="26">
   <si>
     <t>meters</t>
   </si>
@@ -74,6 +74,24 @@
   </si>
   <si>
     <t>Character</t>
+  </si>
+  <si>
+    <t>%5.1f</t>
+  </si>
+  <si>
+    <t>%.3f</t>
+  </si>
+  <si>
+    <t>%.2f</t>
+  </si>
+  <si>
+    <t>%.2e</t>
+  </si>
+  <si>
+    <t>%d</t>
+  </si>
+  <si>
+    <t>%s</t>
   </si>
 </sst>
 </file>
@@ -499,7 +517,7 @@
   <dimension ref="A2:O58"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="P7" sqref="P7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -555,9 +573,7 @@
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B3" s="2" t="s">
-        <v>15</v>
-      </c>
+      <c r="B3" s="2"/>
       <c r="C3" s="2" t="s">
         <v>0</v>
       </c>
@@ -587,32 +603,36 @@
       <c r="O3" s="2"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B4" s="3"/>
-      <c r="C4" s="3">
-        <v>1</v>
-      </c>
-      <c r="D4" s="3">
-        <v>1</v>
-      </c>
-      <c r="E4" s="3">
-        <v>3</v>
-      </c>
-      <c r="F4" s="3">
-        <v>2</v>
-      </c>
-      <c r="G4" s="3">
-        <v>2</v>
-      </c>
-      <c r="H4" s="3">
-        <v>3</v>
+      <c r="B4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3" t="s">
+        <v>23</v>
       </c>
       <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
+      <c r="J4" s="3" t="s">
+        <v>24</v>
+      </c>
       <c r="K4" s="3"/>
       <c r="L4" s="3"/>
       <c r="M4" s="3"/>
       <c r="N4" s="3"/>
-      <c r="O4" s="3"/>
+      <c r="O4" s="3" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="16">

</xml_diff>

<commit_message>
Format header line now comes first
</commit_message>
<xml_diff>
--- a/inst/extdata/DataExample.xlsx
+++ b/inst/extdata/DataExample.xlsx
@@ -504,7 +504,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:O58"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -524,75 +526,75 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
+      <c r="M2" s="2"/>
+      <c r="N2" s="2"/>
+      <c r="O2" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C3" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="G3" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1" t="s">
+      <c r="H3" s="1"/>
+      <c r="I3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="J3" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="K2" s="1"/>
-      <c r="L2" s="1" t="s">
+      <c r="K3" s="1"/>
+      <c r="L3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="M2" s="1" t="s">
+      <c r="M3" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="N2" s="1" t="s">
+      <c r="N3" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="O2" s="1" t="s">
+      <c r="O3" s="1" t="s">
         <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B3" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="I3" s="2"/>
-      <c r="J3" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="K3" s="2"/>
-      <c r="L3" s="2"/>
-      <c r="M3" s="2"/>
-      <c r="N3" s="2"/>
-      <c r="O3" s="2" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Changed a single cell value, adding more digits
</commit_message>
<xml_diff>
--- a/inst/extdata/DataExample.xlsx
+++ b/inst/extdata/DataExample.xlsx
@@ -89,10 +89,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="mm/dd/yyyy\ hh:mm:ss.000"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
     <numFmt numFmtId="166" formatCode="0.000"/>
+    <numFmt numFmtId="169" formatCode="0.000000"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -157,7 +158,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -192,6 +193,9 @@
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -505,7 +509,7 @@
   <dimension ref="A2:O58"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1305,8 +1309,8 @@
       <c r="D21" s="4">
         <v>-9.8000000000000007</v>
       </c>
-      <c r="E21" s="5">
-        <v>2.2867000000000002</v>
+      <c r="E21" s="19">
+        <v>3.1415929999999999</v>
       </c>
       <c r="F21" s="6">
         <v>999.63</v>

</xml_diff>

<commit_message>
Still working on POSIXct format
</commit_message>
<xml_diff>
--- a/inst/extdata/DataExample.xlsx
+++ b/inst/extdata/DataExample.xlsx
@@ -38,9 +38,6 @@
   </si>
   <si>
     <t>T POSIXct</t>
-  </si>
-  <si>
-    <t>%m/%d/%Y %H:%M:%OS</t>
   </si>
   <si>
     <t>Character</t>
@@ -84,6 +81,9 @@
   <si>
     <t>Time character</t>
   </si>
+  <si>
+    <t>%m/%d/%Y %H:%M:%OS3</t>
+  </si>
 </sst>
 </file>
 
@@ -93,7 +93,7 @@
     <numFmt numFmtId="164" formatCode="mm/dd/yyyy\ hh:mm:ss.000"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
     <numFmt numFmtId="166" formatCode="0.000"/>
-    <numFmt numFmtId="169" formatCode="0.000000"/>
+    <numFmt numFmtId="167" formatCode="0.000000"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -194,7 +194,7 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -508,14 +508,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:O58"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="12.42578125" bestFit="1" customWidth="1"/>
@@ -531,34 +529,34 @@
   <sheetData>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>11</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>12</v>
       </c>
       <c r="G2" s="2"/>
       <c r="H2" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I2" s="2"/>
       <c r="J2" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="K2" s="2"/>
       <c r="L2" s="2"/>
       <c r="M2" s="2"/>
       <c r="N2" s="2"/>
       <c r="O2" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
@@ -566,39 +564,39 @@
         <v>7</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="F3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>19</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>20</v>
       </c>
       <c r="H3" s="1"/>
       <c r="I3" s="1" t="s">
         <v>6</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K3" s="1"/>
       <c r="L3" s="1" t="s">
         <v>6</v>
       </c>
       <c r="M3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="N3" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="N3" s="1" t="s">
-        <v>22</v>
-      </c>
       <c r="O3" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Fixed bug that was preventing imports from paste operation
</commit_message>
<xml_diff>
--- a/inst/extdata/DataExample.xlsx
+++ b/inst/extdata/DataExample.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="22">
   <si>
     <t>A1</t>
   </si>
@@ -44,9 +44,6 @@
   </si>
   <si>
     <t>%5.1f</t>
-  </si>
-  <si>
-    <t>%.3f</t>
   </si>
   <si>
     <t>%.2f</t>
@@ -82,7 +79,7 @@
     <t>Time character</t>
   </si>
   <si>
-    <t>%m/%d/%Y %H:%M:%OS3</t>
+    <t>%m/%d/%Y %H:%M:%OS2</t>
   </si>
 </sst>
 </file>
@@ -93,7 +90,7 @@
     <numFmt numFmtId="164" formatCode="mm/dd/yyyy\ hh:mm:ss.000"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
     <numFmt numFmtId="166" formatCode="0.000"/>
-    <numFmt numFmtId="167" formatCode="0.000000"/>
+    <numFmt numFmtId="167" formatCode="0.00000000000"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -194,9 +191,7 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -514,7 +509,7 @@
   <cols>
     <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="24.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.7109375" bestFit="1" customWidth="1"/>
@@ -529,7 +524,7 @@
   <sheetData>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>9</v>
@@ -541,22 +536,22 @@
         <v>10</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G2" s="2"/>
       <c r="H2" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="I2" s="2"/>
       <c r="J2" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="K2" s="2"/>
       <c r="L2" s="2"/>
       <c r="M2" s="2"/>
       <c r="N2" s="2"/>
       <c r="O2" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
@@ -564,36 +559,36 @@
         <v>7</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="F3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>18</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>19</v>
       </c>
       <c r="H3" s="1"/>
       <c r="I3" s="1" t="s">
         <v>6</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="K3" s="1"/>
       <c r="L3" s="1" t="s">
         <v>6</v>
       </c>
       <c r="M3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="N3" s="1" t="s">
         <v>20</v>
-      </c>
-      <c r="N3" s="1" t="s">
-        <v>21</v>
       </c>
       <c r="O3" s="1" t="s">
         <v>8</v>
@@ -733,8 +728,8 @@
       <c r="B7" s="3">
         <v>39927.535409918979</v>
       </c>
-      <c r="C7" s="4">
-        <v>3.7</v>
+      <c r="C7" s="19">
+        <v>3.14159265358979</v>
       </c>
       <c r="D7" s="4">
         <v>-2.2999999999999998</v>
@@ -835,7 +830,7 @@
         <v>4.2999999999999997E-2</v>
       </c>
       <c r="H9" s="8">
-        <v>4.2999999999999997E-2</v>
+        <v>4.2999999999999999E-4</v>
       </c>
       <c r="I9" s="9" t="b">
         <v>1</v>
@@ -846,7 +841,7 @@
       <c r="K9" s="9"/>
       <c r="L9" s="9"/>
       <c r="M9" s="11">
-        <v>39680</v>
+        <v>39681</v>
       </c>
       <c r="N9" s="12">
         <v>0.49805555555555553</v>
@@ -887,7 +882,7 @@
       <c r="K10" s="9"/>
       <c r="L10" s="9"/>
       <c r="M10" s="11">
-        <v>39680</v>
+        <v>39682</v>
       </c>
       <c r="N10" s="12">
         <v>0.49805555555555553</v>
@@ -930,7 +925,7 @@
       <c r="K11" s="9"/>
       <c r="L11" s="9"/>
       <c r="M11" s="11">
-        <v>39680</v>
+        <v>39683</v>
       </c>
       <c r="N11" s="12">
         <v>0.49805555555555553</v>
@@ -971,7 +966,7 @@
       <c r="K12" s="9"/>
       <c r="L12" s="9"/>
       <c r="M12" s="11">
-        <v>39680</v>
+        <v>39684</v>
       </c>
       <c r="N12" s="12">
         <v>0.49805555555555553</v>
@@ -1001,7 +996,7 @@
         <v>4</v>
       </c>
       <c r="H13" s="8">
-        <v>2.9000000000000001E-2</v>
+        <v>2.8999999999999998E-3</v>
       </c>
       <c r="I13" s="9" t="b">
         <v>0</v>
@@ -1012,7 +1007,7 @@
       <c r="K13" s="9"/>
       <c r="L13" s="9"/>
       <c r="M13" s="11">
-        <v>39680</v>
+        <v>39685</v>
       </c>
       <c r="N13" s="12">
         <v>0.49805555555555553</v>
@@ -1055,7 +1050,7 @@
       <c r="K14" s="9"/>
       <c r="L14" s="9"/>
       <c r="M14" s="11">
-        <v>39680</v>
+        <v>39686</v>
       </c>
       <c r="N14" s="12">
         <v>0.49805555555555553</v>
@@ -1096,7 +1091,7 @@
       <c r="K15" s="9"/>
       <c r="L15" s="9"/>
       <c r="M15" s="11">
-        <v>39680</v>
+        <v>39687</v>
       </c>
       <c r="N15" s="12">
         <v>0.49805555555555553</v>
@@ -1139,7 +1134,7 @@
       <c r="K16" s="9"/>
       <c r="L16" s="9"/>
       <c r="M16" s="11">
-        <v>39680</v>
+        <v>39688</v>
       </c>
       <c r="N16" s="12">
         <v>0.49805555555555553</v>
@@ -1182,7 +1177,7 @@
       <c r="K17" s="9"/>
       <c r="L17" s="9"/>
       <c r="M17" s="11">
-        <v>39680</v>
+        <v>39689</v>
       </c>
       <c r="N17" s="12">
         <v>0.49805555555555553</v>
@@ -1225,7 +1220,7 @@
       <c r="K18" s="9"/>
       <c r="L18" s="9"/>
       <c r="M18" s="11">
-        <v>39680</v>
+        <v>39690</v>
       </c>
       <c r="N18" s="12">
         <v>0.49805555555555553</v>
@@ -1266,7 +1261,7 @@
       <c r="K19" s="9"/>
       <c r="L19" s="9"/>
       <c r="M19" s="11">
-        <v>39680</v>
+        <v>39691</v>
       </c>
       <c r="N19" s="12">
         <v>0.49965277777777778</v>
@@ -1307,7 +1302,7 @@
       <c r="D21" s="4">
         <v>-9.8000000000000007</v>
       </c>
-      <c r="E21" s="19">
+      <c r="E21" s="5">
         <v>3.1415929999999999</v>
       </c>
       <c r="F21" s="6">
@@ -1328,7 +1323,7 @@
       <c r="K21" s="9"/>
       <c r="L21" s="9"/>
       <c r="M21" s="11">
-        <v>39680</v>
+        <v>39692</v>
       </c>
       <c r="N21" s="12">
         <v>0.49965277777777778</v>
@@ -1367,7 +1362,7 @@
       <c r="K22" s="9"/>
       <c r="L22" s="9"/>
       <c r="M22" s="11">
-        <v>39680</v>
+        <v>39693</v>
       </c>
       <c r="N22" s="12">
         <v>0.49965277777777778</v>
@@ -1406,7 +1401,7 @@
       <c r="K23" s="9"/>
       <c r="L23" s="9"/>
       <c r="M23" s="11">
-        <v>39680</v>
+        <v>39694</v>
       </c>
       <c r="N23" s="12">
         <v>0.49965277777777778</v>
@@ -1449,7 +1444,7 @@
       <c r="K24" s="9"/>
       <c r="L24" s="9"/>
       <c r="M24" s="11">
-        <v>39680</v>
+        <v>39695</v>
       </c>
       <c r="N24" s="12">
         <v>0.49965277777777778</v>
@@ -1492,7 +1487,7 @@
       <c r="K25" s="9"/>
       <c r="L25" s="9"/>
       <c r="M25" s="11">
-        <v>39680</v>
+        <v>39696</v>
       </c>
       <c r="N25" s="12">
         <v>0.49965277777777778</v>
@@ -1533,7 +1528,7 @@
       <c r="K26" s="9"/>
       <c r="L26" s="9"/>
       <c r="M26" s="11">
-        <v>39680</v>
+        <v>39697</v>
       </c>
       <c r="N26" s="12">
         <v>0.49965277777777778</v>
@@ -1563,7 +1558,7 @@
         <v>-0.85399999999999998</v>
       </c>
       <c r="H27" s="8">
-        <v>-0.754</v>
+        <v>-7.54E-7</v>
       </c>
       <c r="I27" s="9" t="b">
         <v>0</v>
@@ -1574,7 +1569,7 @@
       <c r="K27" s="9"/>
       <c r="L27" s="9"/>
       <c r="M27" s="11">
-        <v>39680</v>
+        <v>39698</v>
       </c>
       <c r="N27" s="12">
         <v>0.49965277777777778</v>
@@ -1615,7 +1610,7 @@
       <c r="K28" s="9"/>
       <c r="L28" s="9"/>
       <c r="M28" s="11">
-        <v>39680</v>
+        <v>39699</v>
       </c>
       <c r="N28" s="12">
         <v>0.49965277777777778</v>
@@ -1658,7 +1653,7 @@
       <c r="K29" s="9"/>
       <c r="L29" s="9"/>
       <c r="M29" s="11">
-        <v>39680</v>
+        <v>39700</v>
       </c>
       <c r="N29" s="12">
         <v>0.49965277777777778</v>
@@ -1699,7 +1694,7 @@
       <c r="K30" s="9"/>
       <c r="L30" s="9"/>
       <c r="M30" s="11">
-        <v>39680</v>
+        <v>39701</v>
       </c>
       <c r="N30" s="12">
         <v>0.49965277777777778</v>
@@ -1740,7 +1735,7 @@
       <c r="K31" s="9"/>
       <c r="L31" s="9"/>
       <c r="M31" s="11">
-        <v>39680</v>
+        <v>39702</v>
       </c>
       <c r="N31" s="12">
         <v>0.49965277777777778</v>
@@ -1783,7 +1778,7 @@
       <c r="K32" s="9"/>
       <c r="L32" s="9"/>
       <c r="M32" s="11">
-        <v>39680</v>
+        <v>39703</v>
       </c>
       <c r="N32" s="12">
         <v>0.50118055555555563</v>
@@ -1824,7 +1819,7 @@
       <c r="K33" s="9"/>
       <c r="L33" s="9"/>
       <c r="M33" s="11">
-        <v>39680</v>
+        <v>39704</v>
       </c>
       <c r="N33" s="12">
         <v>0.50118055555555563</v>
@@ -1865,7 +1860,7 @@
       <c r="K34" s="9"/>
       <c r="L34" s="9"/>
       <c r="M34" s="11">
-        <v>39680</v>
+        <v>39705</v>
       </c>
       <c r="N34" s="12">
         <v>0.50118055555555563</v>
@@ -1906,7 +1901,7 @@
       <c r="K35" s="9"/>
       <c r="L35" s="9"/>
       <c r="M35" s="11">
-        <v>39680</v>
+        <v>39706</v>
       </c>
       <c r="N35" s="12">
         <v>0.50118055555555563</v>
@@ -1947,7 +1942,7 @@
       <c r="K36" s="9"/>
       <c r="L36" s="9"/>
       <c r="M36" s="11">
-        <v>39680</v>
+        <v>39707</v>
       </c>
       <c r="N36" s="12">
         <v>0.50118055555555563</v>
@@ -1988,7 +1983,7 @@
       <c r="K37" s="9"/>
       <c r="L37" s="9"/>
       <c r="M37" s="11">
-        <v>39680</v>
+        <v>39708</v>
       </c>
       <c r="N37" s="12">
         <v>0.50118055555555563</v>
@@ -2029,7 +2024,7 @@
       <c r="K38" s="9"/>
       <c r="L38" s="9"/>
       <c r="M38" s="11">
-        <v>39680</v>
+        <v>39709</v>
       </c>
       <c r="N38" s="12">
         <v>0.50118055555555563</v>
@@ -2070,7 +2065,7 @@
       <c r="K39" s="9"/>
       <c r="L39" s="9"/>
       <c r="M39" s="11">
-        <v>39680</v>
+        <v>39710</v>
       </c>
       <c r="N39" s="12">
         <v>0.50118055555555563</v>
@@ -2111,7 +2106,7 @@
       <c r="K40" s="9"/>
       <c r="L40" s="9"/>
       <c r="M40" s="11">
-        <v>39680</v>
+        <v>39711</v>
       </c>
       <c r="N40" s="12">
         <v>0.50118055555555563</v>
@@ -2152,7 +2147,7 @@
       <c r="K41" s="9"/>
       <c r="L41" s="9"/>
       <c r="M41" s="11">
-        <v>39680</v>
+        <v>39712</v>
       </c>
       <c r="N41" s="12">
         <v>0.50118055555555563</v>
@@ -2195,7 +2190,7 @@
       <c r="K42" s="9"/>
       <c r="L42" s="9"/>
       <c r="M42" s="11">
-        <v>39680</v>
+        <v>39713</v>
       </c>
       <c r="N42" s="12">
         <v>0.50118055555555563</v>
@@ -2236,7 +2231,7 @@
       <c r="K43" s="9"/>
       <c r="L43" s="9"/>
       <c r="M43" s="11">
-        <v>39680</v>
+        <v>39714</v>
       </c>
       <c r="N43" s="12">
         <v>0.50118055555555563</v>
@@ -2277,7 +2272,7 @@
       <c r="K44" s="9"/>
       <c r="L44" s="9"/>
       <c r="M44" s="11">
-        <v>39680</v>
+        <v>39715</v>
       </c>
       <c r="N44" s="12">
         <v>0.50274305555555554</v>
@@ -2318,7 +2313,7 @@
       <c r="K45" s="9"/>
       <c r="L45" s="9"/>
       <c r="M45" s="11">
-        <v>39680</v>
+        <v>39716</v>
       </c>
       <c r="N45" s="12">
         <v>0.50274305555555554</v>
@@ -2359,7 +2354,7 @@
       <c r="K46" s="9"/>
       <c r="L46" s="9"/>
       <c r="M46" s="11">
-        <v>39680</v>
+        <v>39717</v>
       </c>
       <c r="N46" s="12">
         <v>0.50274305555555554</v>
@@ -2400,7 +2395,7 @@
       <c r="K47" s="9"/>
       <c r="L47" s="9"/>
       <c r="M47" s="11">
-        <v>39680</v>
+        <v>39718</v>
       </c>
       <c r="N47" s="12">
         <v>0.50274305555555554</v>
@@ -2443,7 +2438,7 @@
       <c r="K48" s="9"/>
       <c r="L48" s="9"/>
       <c r="M48" s="11">
-        <v>39680</v>
+        <v>39719</v>
       </c>
       <c r="N48" s="12">
         <v>0.50274305555555554</v>
@@ -2484,7 +2479,7 @@
       <c r="K49" s="9"/>
       <c r="L49" s="9"/>
       <c r="M49" s="11">
-        <v>39680</v>
+        <v>39720</v>
       </c>
       <c r="N49" s="12">
         <v>0.50274305555555554</v>
@@ -2525,7 +2520,7 @@
       <c r="K50" s="9"/>
       <c r="L50" s="9"/>
       <c r="M50" s="11">
-        <v>39680</v>
+        <v>39721</v>
       </c>
       <c r="N50" s="12">
         <v>0.50274305555555554</v>
@@ -2568,7 +2563,7 @@
       <c r="K51" s="9"/>
       <c r="L51" s="9"/>
       <c r="M51" s="11">
-        <v>39680</v>
+        <v>39722</v>
       </c>
       <c r="N51" s="12">
         <v>0.50274305555555554</v>
@@ -2611,7 +2606,7 @@
       <c r="K52" s="9"/>
       <c r="L52" s="9"/>
       <c r="M52" s="11">
-        <v>39680</v>
+        <v>39723</v>
       </c>
       <c r="N52" s="12">
         <v>0.50274305555555554</v>
@@ -2652,7 +2647,7 @@
       <c r="K53" s="9"/>
       <c r="L53" s="9"/>
       <c r="M53" s="11">
-        <v>39680</v>
+        <v>39724</v>
       </c>
       <c r="N53" s="12">
         <v>0.50274305555555554</v>
@@ -2693,7 +2688,7 @@
       <c r="K54" s="9"/>
       <c r="L54" s="9"/>
       <c r="M54" s="11">
-        <v>39680</v>
+        <v>39725</v>
       </c>
       <c r="N54" s="12">
         <v>0.54167824074074067</v>

</xml_diff>